<commit_message>
Colored one line of code
</commit_message>
<xml_diff>
--- a/tests/artifact/script/Account.xlsx
+++ b/tests/artifact/script/Account.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="6950" tabRatio="500" firstSheet="2" activeTab="4"/>
+    <workbookView windowWidth="18350" windowHeight="6950" tabRatio="500" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -2945,7 +2945,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2961,6 +2961,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.0499893185216834"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3309,7 +3315,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3333,16 +3339,16 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -3351,89 +3357,89 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3577,8 +3583,41 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6816,7 +6855,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="5" s="44" customFormat="1" ht="32" customHeight="1" spans="1:16384">
+    <row r="5" s="53" customFormat="1" ht="32" customHeight="1" spans="1:16384">
       <c r="A5" s="20" t="s">
         <v>747</v>
       </c>
@@ -23309,73 +23348,73 @@
       <c r="N9" s="24"/>
       <c r="O9" s="23"/>
     </row>
-    <row r="10" s="45" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A10" s="46"/>
-      <c r="B10" s="47"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="56"/>
-      <c r="K10" s="57"/>
-      <c r="L10" s="58"/>
-      <c r="M10" s="59"/>
-      <c r="N10" s="58"/>
-      <c r="O10" s="57"/>
-    </row>
-    <row r="11" s="45" customFormat="1" ht="19" customHeight="1" spans="1:15">
-      <c r="A11" s="46"/>
-      <c r="B11" s="47"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="49"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="56"/>
-      <c r="K11" s="57"/>
-      <c r="L11" s="58"/>
-      <c r="M11" s="59"/>
-      <c r="N11" s="58"/>
-      <c r="O11" s="57"/>
-    </row>
-    <row r="12" s="45" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A12" s="46"/>
-      <c r="B12" s="47"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="56"/>
-      <c r="K12" s="57"/>
-      <c r="L12" s="58"/>
-      <c r="M12" s="59"/>
-      <c r="N12" s="58"/>
-      <c r="O12" s="57"/>
-    </row>
-    <row r="13" s="45" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A13" s="46"/>
-      <c r="B13" s="47"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="56"/>
-      <c r="K13" s="57"/>
-      <c r="L13" s="58"/>
-      <c r="M13" s="59"/>
-      <c r="N13" s="58"/>
-      <c r="O13" s="57"/>
+    <row r="10" s="54" customFormat="1" ht="23" customHeight="1" spans="1:15">
+      <c r="A10" s="55"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="58"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="65"/>
+      <c r="K10" s="66"/>
+      <c r="L10" s="67"/>
+      <c r="M10" s="68"/>
+      <c r="N10" s="67"/>
+      <c r="O10" s="66"/>
+    </row>
+    <row r="11" s="54" customFormat="1" ht="19" customHeight="1" spans="1:15">
+      <c r="A11" s="55"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="58"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="65"/>
+      <c r="K11" s="66"/>
+      <c r="L11" s="67"/>
+      <c r="M11" s="68"/>
+      <c r="N11" s="67"/>
+      <c r="O11" s="66"/>
+    </row>
+    <row r="12" s="54" customFormat="1" ht="23" customHeight="1" spans="1:15">
+      <c r="A12" s="55"/>
+      <c r="B12" s="56"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="65"/>
+      <c r="K12" s="66"/>
+      <c r="L12" s="67"/>
+      <c r="M12" s="68"/>
+      <c r="N12" s="67"/>
+      <c r="O12" s="66"/>
+    </row>
+    <row r="13" s="54" customFormat="1" ht="23" customHeight="1" spans="1:15">
+      <c r="A13" s="55"/>
+      <c r="B13" s="56"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="65"/>
+      <c r="K13" s="66"/>
+      <c r="L13" s="67"/>
+      <c r="M13" s="68"/>
+      <c r="N13" s="67"/>
+      <c r="O13" s="66"/>
     </row>
     <row r="14" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A14" s="20"/>
@@ -23498,7 +23537,7 @@
     </row>
     <row r="21" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A21" s="20"/>
-      <c r="B21" s="55"/>
+      <c r="B21" s="64"/>
       <c r="C21" s="26"/>
       <c r="D21" s="27"/>
       <c r="E21" s="27"/>
@@ -26495,8 +26534,8 @@
   <sheetPr/>
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D2"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A11" sqref="$A11:$XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
@@ -26677,7 +26716,7 @@
       <c r="F6" s="28" t="s">
         <v>764</v>
       </c>
-      <c r="G6" s="42"/>
+      <c r="G6" s="43"/>
       <c r="H6" s="27"/>
       <c r="I6" s="27"/>
       <c r="J6" s="28"/>
@@ -26906,7 +26945,7 @@
       <c r="D15" s="27"/>
       <c r="E15" s="27"/>
       <c r="F15" s="28"/>
-      <c r="G15" s="42"/>
+      <c r="G15" s="43"/>
       <c r="H15" s="27"/>
       <c r="I15" s="27"/>
       <c r="J15" s="28"/>
@@ -27690,7 +27729,7 @@
       <c r="E14" s="30" t="s">
         <v>756</v>
       </c>
-      <c r="F14" s="43"/>
+      <c r="F14" s="52"/>
       <c r="G14" s="30"/>
       <c r="H14" s="27"/>
       <c r="I14" s="27"/>
@@ -29834,8 +29873,8 @@
   <sheetPr/>
   <dimension ref="A1:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D2"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
@@ -29989,7 +30028,7 @@
       <c r="F5" s="28" t="s">
         <v>764</v>
       </c>
-      <c r="G5" s="42"/>
+      <c r="G5" s="43"/>
       <c r="H5" s="27"/>
       <c r="I5" s="27"/>
       <c r="J5" s="28"/>
@@ -30150,7 +30189,7 @@
       <c r="F11" s="28" t="s">
         <v>764</v>
       </c>
-      <c r="G11" s="42"/>
+      <c r="G11" s="43"/>
       <c r="H11" s="27"/>
       <c r="I11" s="27"/>
       <c r="J11" s="28"/>
@@ -30285,7 +30324,7 @@
       <c r="F16" s="28" t="s">
         <v>806</v>
       </c>
-      <c r="G16" s="42"/>
+      <c r="G16" s="43"/>
       <c r="H16" s="27"/>
       <c r="I16" s="27"/>
       <c r="J16" s="28"/>
@@ -30372,34 +30411,34 @@
       <c r="N19" s="24"/>
       <c r="O19" s="23"/>
     </row>
-    <row r="20" s="2" customFormat="1" ht="42" spans="1:15">
-      <c r="A20" s="20" t="s">
+    <row r="20" s="42" customFormat="1" ht="42" spans="1:15">
+      <c r="A20" s="44" t="s">
         <v>808</v>
       </c>
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="45" t="s">
         <v>803</v>
       </c>
-      <c r="C20" s="29" t="s">
+      <c r="C20" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="30" t="s">
+      <c r="D20" s="47" t="s">
         <v>263</v>
       </c>
-      <c r="E20" s="30" t="s">
+      <c r="E20" s="47" t="s">
         <v>756</v>
       </c>
-      <c r="F20" s="30" t="s">
+      <c r="F20" s="47" t="s">
         <v>761</v>
       </c>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="27"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="23"/>
-      <c r="L20" s="24"/>
-      <c r="M20" s="22"/>
-      <c r="N20" s="24"/>
-      <c r="O20" s="23"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="47"/>
+      <c r="I20" s="47"/>
+      <c r="J20" s="48"/>
+      <c r="K20" s="49"/>
+      <c r="L20" s="50"/>
+      <c r="M20" s="51"/>
+      <c r="N20" s="50"/>
+      <c r="O20" s="49"/>
     </row>
     <row r="21" s="2" customFormat="1" ht="39" customHeight="1" spans="2:15">
       <c r="B21" s="21" t="s">
@@ -30417,7 +30456,7 @@
       <c r="F21" s="28" t="s">
         <v>806</v>
       </c>
-      <c r="G21" s="42"/>
+      <c r="G21" s="43"/>
       <c r="H21" s="27"/>
       <c r="I21" s="27"/>
       <c r="J21" s="28"/>
@@ -30498,7 +30537,7 @@
       <c r="F24" s="28" t="s">
         <v>764</v>
       </c>
-      <c r="G24" s="42"/>
+      <c r="G24" s="43"/>
       <c r="H24" s="27"/>
       <c r="I24" s="27"/>
       <c r="J24" s="28"/>
@@ -30915,7 +30954,7 @@
       <c r="F40" s="28" t="s">
         <v>777</v>
       </c>
-      <c r="G40" s="42"/>
+      <c r="G40" s="43"/>
       <c r="H40" s="27"/>
       <c r="I40" s="27"/>
       <c r="J40" s="28"/>
@@ -31273,10 +31312,10 @@
   <sheetPr/>
   <dimension ref="A1:O180"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:D2"/>
+      <selection pane="bottomLeft" activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>

</xml_diff>